<commit_message>
Release version 1.42 - Miner configuration worker, controllers, new commands, file extensions.
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="311">
   <si>
     <t>№</t>
   </si>
@@ -949,6 +949,24 @@
   </si>
   <si>
     <t>Invalid certificate excahange</t>
+  </si>
+  <si>
+    <t>Invalid digital address of operator</t>
+  </si>
+  <si>
+    <t>Imported configration</t>
+  </si>
+  <si>
+    <t>New Contact Added</t>
+  </si>
+  <si>
+    <t>New Operator Added</t>
+  </si>
+  <si>
+    <t>Created New configration file</t>
+  </si>
+  <si>
+    <t>DNS Updated</t>
   </si>
 </sst>
 </file>
@@ -1397,9 +1415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1503,7 @@
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(C2,":{",J2,J3,J4,J5,J6,J7,J8,J9,J10,J11,J12,J13,J14,J15,J16,J17,J18,J19,J20,J21,"},")</f>
-        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
+        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
       </c>
       <c r="L2" t="str">
         <f>CONCATENATE(I2,":'pPort is NOT connected'",",")</f>
@@ -1693,7 +1711,7 @@
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>203</v>
@@ -1731,15 +1749,19 @@
       <c r="F9" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>305</v>
+      </c>
       <c r="I9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>pPort_Err0008</v>
       </c>
       <c r="J9" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>Err0008:{str:'', data: tablePorts.pPort_Err0008},</v>
+        <v>Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="2"/>
@@ -3170,7 +3192,7 @@
       </c>
       <c r="K52" t="str">
         <f>CONCATENATE(C52,":{",J52,J53,J54,J55,J56,J57,J58,J59,J60,J61,J62,J63,J64,J65,J66,J67,J68,J69,J70,J71,J72,J73,J74,J75,J76,J77,J78,J79,J80,J81,J82,J83,J84,J85,J86,J87,J88,J89,J90,J91,J92,J93,J94,J95,J96,J97,J98,J99,J100,J101,J102,J103,J104,J105,J106,J107,J108,J109,J110,J111,"},")</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="2"/>
@@ -4382,15 +4404,19 @@
       <c r="F86" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G86" s="18"/>
-      <c r="H86" s="9"/>
+      <c r="G86" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="I86" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0085</v>
       </c>
       <c r="J86" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0085:{str:'', data: tablePorts.pPort_UsInf0085},</v>
+        <v>UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},</v>
       </c>
       <c r="L86" t="str">
         <f t="shared" si="6"/>
@@ -4414,15 +4440,19 @@
       <c r="F87" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G87" s="18"/>
-      <c r="H87" s="9"/>
+      <c r="G87" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H87" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="I87" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0086</v>
       </c>
       <c r="J87" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0086:{str:'', data: tablePorts.pPort_UsInf0086},</v>
+        <v>UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},</v>
       </c>
       <c r="L87" t="str">
         <f t="shared" si="6"/>
@@ -4446,15 +4476,19 @@
       <c r="F88" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G88" s="18"/>
-      <c r="H88" s="15"/>
+      <c r="G88" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H88" s="15" t="s">
+        <v>308</v>
+      </c>
       <c r="I88" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0087</v>
       </c>
       <c r="J88" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0087:{str:'', data: tablePorts.pPort_UsInf0087},</v>
+        <v>UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},</v>
       </c>
       <c r="L88" t="str">
         <f t="shared" si="6"/>
@@ -4478,15 +4512,19 @@
       <c r="F89" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G89" s="18"/>
-      <c r="H89" s="15"/>
+      <c r="G89" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>309</v>
+      </c>
       <c r="I89" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0088</v>
       </c>
       <c r="J89" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0088:{str:'', data: tablePorts.pPort_UsInf0088},</v>
+        <v>UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},</v>
       </c>
       <c r="L89" t="str">
         <f t="shared" si="6"/>
@@ -4510,15 +4548,19 @@
       <c r="F90" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G90" s="18"/>
-      <c r="H90" s="15"/>
+      <c r="G90" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H90" s="15" t="s">
+        <v>310</v>
+      </c>
       <c r="I90" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0089</v>
       </c>
       <c r="J90" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0089:{str:'', data: tablePorts.pPort_UsInf0089},</v>
+        <v>UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},</v>
       </c>
       <c r="L90" t="str">
         <f t="shared" si="6"/>
@@ -5937,7 +5979,7 @@
   <dimension ref="A1:A149"/>
   <sheetViews>
     <sheetView topLeftCell="A143" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167:A168"/>
+      <selection activeCell="A145" sqref="A145:A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6766,7 +6808,7 @@
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="str">
         <f>CodeTable_Single_data!K2</f>
-        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
+        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
@@ -6778,7 +6820,7 @@
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
         <f>CodeTable_Single_data!K52</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Software version 1.45. Listing of units, obfustication, balance
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="312">
   <si>
     <t>№</t>
   </si>
@@ -967,6 +967,9 @@
   </si>
   <si>
     <t>DNS Updated</t>
+  </si>
+  <si>
+    <t>Balance %s</t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1419,8 @@
   <dimension ref="A1:L138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3195,7 @@
       </c>
       <c r="K52" t="str">
         <f>CONCATENATE(C52,":{",J52,J53,J54,J55,J56,J57,J58,J59,J60,J61,J62,J63,J64,J65,J66,J67,J68,J69,J70,J71,J72,J73,J74,J75,J76,J77,J78,J79,J80,J81,J82,J83,J84,J85,J86,J87,J88,J89,J90,J91,J92,J93,J94,J95,J96,J97,J98,J99,J100,J101,J102,J103,J104,J105,J106,J107,J108,J109,J110,J111,"},")</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="2"/>
@@ -4584,15 +4587,19 @@
       <c r="F91" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G91" s="18"/>
-      <c r="H91" s="15"/>
+      <c r="G91" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H91" s="15" t="s">
+        <v>311</v>
+      </c>
       <c r="I91" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0090</v>
       </c>
       <c r="J91" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},</v>
+        <v>UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},</v>
       </c>
       <c r="L91" t="str">
         <f t="shared" si="6"/>
@@ -6820,7 +6827,7 @@
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
         <f>CodeTable_Single_data!K52</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Release version - 1.46 - Scrapping
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="313">
   <si>
     <t>№</t>
   </si>
@@ -970,6 +970,9 @@
   </si>
   <si>
     <t>Balance %s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICE Scrapped unit successfully registered </t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1422,8 @@
   <dimension ref="A1:L138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H96" sqref="H96"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3195,7 +3198,7 @@
       </c>
       <c r="K52" t="str">
         <f>CONCATENATE(C52,":{",J52,J53,J54,J55,J56,J57,J58,J59,J60,J61,J62,J63,J64,J65,J66,J67,J68,J69,J70,J71,J72,J73,J74,J75,J76,J77,J78,J79,J80,J81,J82,J83,J84,J85,J86,J87,J88,J89,J90,J91,J92,J93,J94,J95,J96,J97,J98,J99,J100,J101,J102,J103,J104,J105,J106,J107,J108,J109,J110,J111,"},")</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="2"/>
@@ -4405,7 +4408,7 @@
       </c>
       <c r="E86" s="17"/>
       <c r="F86" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G86" s="18" t="s">
         <v>175</v>
@@ -4441,7 +4444,7 @@
       </c>
       <c r="E87" s="17"/>
       <c r="F87" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G87" s="18" t="s">
         <v>175</v>
@@ -4477,7 +4480,7 @@
       </c>
       <c r="E88" s="17"/>
       <c r="F88" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G88" s="18" t="s">
         <v>175</v>
@@ -4513,7 +4516,7 @@
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G89" s="18" t="s">
         <v>175</v>
@@ -4549,7 +4552,7 @@
       </c>
       <c r="E90" s="17"/>
       <c r="F90" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G90" s="18" t="s">
         <v>175</v>
@@ -4585,7 +4588,7 @@
       </c>
       <c r="E91" s="17"/>
       <c r="F91" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G91" s="18" t="s">
         <v>175</v>
@@ -4621,17 +4624,21 @@
       </c>
       <c r="E92" s="17"/>
       <c r="F92" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G92" s="18"/>
-      <c r="H92" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="G92" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>312</v>
+      </c>
       <c r="I92" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0091</v>
       </c>
       <c r="J92" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},</v>
+        <v>UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},</v>
       </c>
       <c r="L92" t="str">
         <f t="shared" si="6"/>
@@ -5986,7 +5993,7 @@
   <dimension ref="A1:A149"/>
   <sheetViews>
     <sheetView topLeftCell="A143" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145:A148"/>
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6827,7 +6834,7 @@
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
         <f>CodeTable_Single_data!K52</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Release version - 1.46 Patch 1
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -1421,9 +1421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Release version - 1.48 - Global Threshold and UNIT testing
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="315">
   <si>
     <t>№</t>
   </si>
@@ -973,6 +973,12 @@
   </si>
   <si>
     <t xml:space="preserve">DICE Scrapped unit successfully registered </t>
+  </si>
+  <si>
+    <t>There is no active MySQL server on %s</t>
+  </si>
+  <si>
+    <t>Updating from cloud FAILED</t>
   </si>
 </sst>
 </file>
@@ -1422,8 +1428,8 @@
   <dimension ref="A1:L138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1509,7 +1515,7 @@
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(C2,":{",J2,J3,J4,J5,J6,J7,J8,J9,J10,J11,J12,J13,J14,J15,J16,J17,J18,J19,J20,J21,"},")</f>
-        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
+        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'There is no active MySQL server on %s', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
       </c>
       <c r="L2" t="str">
         <f>CONCATENATE(I2,":'pPort is NOT connected'",",")</f>
@@ -1753,7 +1759,7 @@
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>175</v>
@@ -1789,17 +1795,21 @@
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="9"/>
+        <v>297</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>313</v>
+      </c>
       <c r="I10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>pPort_Err0009</v>
       </c>
       <c r="J10" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>Err0009:{str:'', data: tablePorts.pPort_Err0009},</v>
+        <v>Err0009:{str:'There is no active MySQL server on %s', data: tablePorts.pPort_Err0009},</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="2"/>
@@ -2193,7 +2203,7 @@
       </c>
       <c r="K22" t="str">
         <f>CONCATENATE(C22,":{",J22,J23,J24,J25,J26,J27,J28,J29,J30,J31,J32,J33,J34,J35,J36,J37,J38,J39,J40,J41,J42,J43,J44,J45,J46,J47,J48,J49,J50,J51,"},")</f>
-        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
+        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="2"/>
@@ -2515,17 +2525,21 @@
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>314</v>
+      </c>
       <c r="I31" s="9" t="str">
         <f t="shared" si="0"/>
         <v>pPort_Warn0030</v>
       </c>
       <c r="J31" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>Warn0030:{str:'', data: tablePorts.pPort_Warn0030},</v>
+        <v>Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="2"/>
@@ -5993,7 +6007,7 @@
   <dimension ref="A1:A149"/>
   <sheetViews>
     <sheetView topLeftCell="A143" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+      <selection activeCell="A145" sqref="A145:A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6822,13 +6836,13 @@
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="str">
         <f>CodeTable_Single_data!K2</f>
-        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
+        <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'There is no active MySQL server on %s', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="str">
         <f>CodeTable_Single_data!K22</f>
-        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
+        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add update of view interfaces
related messages to console of Amount trading feature
</commit_message>
<xml_diff>
--- a/docs/ConsoleOutputTable.xlsx
+++ b/docs/ConsoleOutputTable.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_49C293F66CB9A1213DDE034038318CA84AB6BA5A" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{300E969D-FFB9-46A6-A748-1360E64A5DD5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeTable_Single_data" sheetId="3" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="warnings" localSheetId="0">CodeTable_Single_data!#REF!</definedName>
     <definedName name="warnings">CodeTable!$M$12:$M$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179020"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="323">
   <si>
     <t>№</t>
   </si>
@@ -979,12 +980,24 @@
   </si>
   <si>
     <t>Updating from cloud FAILED</t>
+  </si>
+  <si>
+    <t>You want to trade %s mDICE</t>
+  </si>
+  <si>
+    <t>Available units are insufficient for the amount</t>
+  </si>
+  <si>
+    <t>Unable to assemble the exact amount. Possible amount %s mDICE</t>
+  </si>
+  <si>
+    <t>All units are packed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1424,31 +1437,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="12.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.77734375" style="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="16" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.78125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="2"/>
+    <col min="3" max="3" width="12.10546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.76171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.734375" style="16" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.796875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="18.0234375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.21875" customWidth="1"/>
-    <col min="10" max="10" width="100.77734375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="255.77734375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="40" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="53.26953125" customWidth="1"/>
+    <col min="10" max="10" width="100.7578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="255.73046875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="39.953125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1522,7 +1535,7 @@
         <v>pPort_Err0001:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1560,7 +1573,7 @@
         <v>pPort_Err0002:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1598,7 +1611,7 @@
         <v>pPort_Err0003:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>pPort_Err0004:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1672,7 +1685,7 @@
         <v>pPort_Err0005:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1708,7 +1721,7 @@
         <v>pPort_Err0006:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1744,7 +1757,7 @@
         <v>pPort_Err0007:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1780,7 +1793,7 @@
         <v>pPort_Err0008:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1816,7 +1829,7 @@
         <v>pPort_Err0009:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1848,7 +1861,7 @@
         <v>pPort_Err0010:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>pPort_Err0011:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1912,7 +1925,7 @@
         <v>pPort_Err0012:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1944,7 +1957,7 @@
         <v>pPort_Err0013:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1976,7 +1989,7 @@
         <v>pPort_Err0014:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>pPort_Err0015:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -2040,7 +2053,7 @@
         <v>pPort_Err0016:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -2072,7 +2085,7 @@
         <v>pPort_Err0017:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>pPort_Err0018:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -2136,7 +2149,7 @@
         <v>pPort_Err0019:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2168,7 +2181,7 @@
         <v>pPort_Err0020:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2203,14 +2216,14 @@
       </c>
       <c r="K22" t="str">
         <f>CONCATENATE(C22,":{",J22,J23,J24,J25,J26,J27,J28,J29,J30,J31,J32,J33,J34,J35,J36,J37,J38,J39,J40,J41,J42,J43,J44,J45,J46,J47,J48,J49,J50,J51,"},")</f>
-        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
+        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'Available units are insufficient for the amount', data: tablePorts.pPort_Warn0031},Warn0032:{str:'Unable to assemble the exact amount. Possible amount %s mDICE', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="2"/>
         <v>pPort_Warn0021:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -2248,7 +2261,7 @@
         <v>pPort_Warn0022:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -2286,7 +2299,7 @@
         <v>pPort_Warn0023:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2324,7 +2337,7 @@
         <v>pPort_Warn0024:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2362,7 +2375,7 @@
         <v>pPort_Warn0025:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2400,7 +2413,7 @@
         <v>pPort_Warn0026:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -2438,7 +2451,7 @@
         <v>pPort_Warn0027:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2474,7 +2487,7 @@
         <v>pPort_Warn0028:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2510,7 +2523,7 @@
         <v>pPort_Warn0029:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -2546,7 +2559,7 @@
         <v>pPort_Warn0030:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -2561,23 +2574,28 @@
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G32" s="18"/>
+        <v>297</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" t="s">
+        <v>316</v>
+      </c>
       <c r="I32" s="9" t="str">
         <f t="shared" si="0"/>
         <v>pPort_Warn0031</v>
       </c>
       <c r="J32" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>Warn0031:{str:'', data: tablePorts.pPort_Warn0031},</v>
+        <v>Warn0031:{str:'Available units are insufficient for the amount', data: tablePorts.pPort_Warn0031},</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="2"/>
         <v>pPort_Warn0031:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -2592,24 +2610,28 @@
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>317</v>
+      </c>
       <c r="I33" s="9" t="str">
         <f t="shared" si="0"/>
         <v>pPort_Warn0032</v>
       </c>
       <c r="J33" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>Warn0032:{str:'', data: tablePorts.pPort_Warn0032},</v>
+        <v>Warn0032:{str:'Unable to assemble the exact amount. Possible amount %s mDICE', data: tablePorts.pPort_Warn0032},</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="2"/>
         <v>pPort_Warn0032:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -2641,7 +2663,7 @@
         <v>pPort_Warn0033:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -2672,7 +2694,7 @@
         <v>pPort_Warn0034:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -2704,7 +2726,7 @@
         <v>pPort_Warn0035:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -2736,7 +2758,7 @@
         <v>pPort_Warn0036:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2767,7 +2789,7 @@
         <v>pPort_Warn0037:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2799,7 +2821,7 @@
         <v>pPort_Warn0038:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2830,7 +2852,7 @@
         <v>pPort_Warn0039:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2862,7 +2884,7 @@
         <v>pPort_Warn0040:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2894,7 +2916,7 @@
         <v>pPort_Warn0041:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2925,7 +2947,7 @@
         <v>pPort_Warn0042:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -2957,7 +2979,7 @@
         <v>pPort_Warn0043:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -2989,7 +3011,7 @@
         <v>pPort_Warn0044:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -3020,7 +3042,7 @@
         <v>pPort_Warn0045:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -3052,7 +3074,7 @@
         <v>pPort_Warn0046:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -3083,7 +3105,7 @@
         <v>pPort_Warn0047:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -3115,7 +3137,7 @@
         <v>pPort_Warn0048:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -3147,7 +3169,7 @@
         <v>pPort_Warn0049:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -3179,7 +3201,7 @@
         <v>pPort_Warn0050:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -3212,14 +3234,14 @@
       </c>
       <c r="K52" t="str">
         <f>CONCATENATE(C52,":{",J52,J53,J54,J55,J56,J57,J58,J59,J60,J61,J62,J63,J64,J65,J66,J67,J68,J69,J70,J71,J72,J73,J74,J75,J76,J77,J78,J79,J80,J81,J82,J83,J84,J85,J86,J87,J88,J89,J90,J91,J92,J93,J94,J95,J96,J97,J98,J99,J100,J101,J102,J103,J104,J105,J106,J107,J108,J109,J110,J111,"},")</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'You want to trade %s mDICE', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'All units are packed', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="2"/>
         <v>pPort_UsInf0051:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -3255,7 +3277,7 @@
         <v>pPort_UsInf0052:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -3291,7 +3313,7 @@
         <v>pPort_UsInf0053:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -3327,7 +3349,7 @@
         <v>pPort_UsInf0054:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -3363,7 +3385,7 @@
         <v>pPort_UsInf0055:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -3399,7 +3421,7 @@
         <v>pPort_UsInf0056:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -3435,7 +3457,7 @@
         <v>pPort_UsInf0057:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -3471,7 +3493,7 @@
         <v>pPort_UsInf0058:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -3507,7 +3529,7 @@
         <v>pPort_UsInf0059:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -3543,7 +3565,7 @@
         <v>pPort_UsInf0060:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -3579,7 +3601,7 @@
         <v>pPort_UsInf0061:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -3615,7 +3637,7 @@
         <v>pPort_UsInf0062:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -3651,7 +3673,7 @@
         <v>pPort_UsInf0063:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -3687,7 +3709,7 @@
         <v>pPort_UsInf0064:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -3723,7 +3745,7 @@
         <v>pPort_UsInf0065:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -3759,7 +3781,7 @@
         <v>pPort_UsInf0066:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -3795,7 +3817,7 @@
         <v>pPort_UsInf0067:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -3831,7 +3853,7 @@
         <v>pPort_UsInf0068:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -3867,7 +3889,7 @@
         <v>pPort_UsInf0069:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -3903,7 +3925,7 @@
         <v>pPort_UsInf0070:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -3939,7 +3961,7 @@
         <v>pPort_UsInf0071:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -3975,7 +3997,7 @@
         <v>pPort_UsInf0072:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -4011,7 +4033,7 @@
         <v>pPort_UsInf0073:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -4047,7 +4069,7 @@
         <v>pPort_UsInf0074:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -4083,7 +4105,7 @@
         <v>pPort_UsInf0075:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -4119,7 +4141,7 @@
         <v>pPort_UsInf0076:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -4155,7 +4177,7 @@
         <v>pPort_UsInf0077:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -4191,7 +4213,7 @@
         <v>pPort_UsInf0078:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -4227,7 +4249,7 @@
         <v>pPort_UsInf0079:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -4263,7 +4285,7 @@
         <v>pPort_UsInf0080:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -4299,7 +4321,7 @@
         <v>pPort_UsInf0081:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -4335,7 +4357,7 @@
         <v>pPort_UsInf0082:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -4371,7 +4393,7 @@
         <v>pPort_UsInf0083:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -4407,7 +4429,7 @@
         <v>pPort_UsInf0084:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -4443,7 +4465,7 @@
         <v>pPort_UsInf0085:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -4479,7 +4501,7 @@
         <v>pPort_UsInf0086:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -4515,7 +4537,7 @@
         <v>pPort_UsInf0087:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -4551,7 +4573,7 @@
         <v>pPort_UsInf0088:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -4587,7 +4609,7 @@
         <v>pPort_UsInf0089:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -4623,7 +4645,7 @@
         <v>pPort_UsInf0090:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -4659,7 +4681,7 @@
         <v>pPort_UsInf0091:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -4674,24 +4696,28 @@
       </c>
       <c r="E93" s="17"/>
       <c r="F93" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G93" s="18"/>
-      <c r="H93" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="G93" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H93" s="15" t="s">
+        <v>315</v>
+      </c>
       <c r="I93" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0092</v>
       </c>
       <c r="J93" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},</v>
+        <v>UsInf0092:{str:'You want to trade %s mDICE', data: tablePorts.pPort_UsInf0092},</v>
       </c>
       <c r="L93" t="str">
         <f t="shared" si="6"/>
         <v>pPort_UsInf0092:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -4706,24 +4732,28 @@
       </c>
       <c r="E94" s="17"/>
       <c r="F94" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G94" s="18"/>
-      <c r="H94" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="G94" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H94" s="15" t="s">
+        <v>318</v>
+      </c>
       <c r="I94" s="9" t="str">
         <f t="shared" si="5"/>
         <v>pPort_UsInf0093</v>
       </c>
       <c r="J94" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},</v>
+        <v>UsInf0093:{str:'All units are packed', data: tablePorts.pPort_UsInf0093},</v>
       </c>
       <c r="L94" t="str">
         <f t="shared" si="6"/>
         <v>pPort_UsInf0093:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -4755,7 +4785,7 @@
         <v>pPort_UsInf0094:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -4787,7 +4817,7 @@
         <v>pPort_UsInf0095:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -4819,7 +4849,7 @@
         <v>pPort_UsInf0096:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -4851,7 +4881,7 @@
         <v>pPort_UsInf0097:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -4883,7 +4913,7 @@
         <v>pPort_UsInf0098:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -4915,7 +4945,7 @@
         <v>pPort_UsInf0099:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>100</v>
       </c>
@@ -4947,7 +4977,7 @@
         <v>pPort_UsInf0100:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>101</v>
       </c>
@@ -4979,7 +5009,7 @@
         <v>pPort_UsInf0101:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>102</v>
       </c>
@@ -5011,7 +5041,7 @@
         <v>pPort_UsInf0102:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>103</v>
       </c>
@@ -5043,7 +5073,7 @@
         <v>pPort_UsInf0103:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>104</v>
       </c>
@@ -5075,7 +5105,7 @@
         <v>pPort_UsInf0104:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>105</v>
       </c>
@@ -5107,7 +5137,7 @@
         <v>pPort_UsInf0105:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
         <v>106</v>
       </c>
@@ -5139,7 +5169,7 @@
         <v>pPort_UsInf0106:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
         <v>107</v>
       </c>
@@ -5171,7 +5201,7 @@
         <v>pPort_UsInf0107:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>108</v>
       </c>
@@ -5203,7 +5233,7 @@
         <v>pPort_UsInf0108:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>109</v>
       </c>
@@ -5235,7 +5265,7 @@
         <v>pPort_UsInf0109:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
         <v>110</v>
       </c>
@@ -5267,7 +5297,7 @@
         <v>pPort_UsInf0110:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>111</v>
       </c>
@@ -5309,7 +5339,7 @@
         <v>pPort_DevInf0111:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>112</v>
       </c>
@@ -5347,7 +5377,7 @@
         <v>pPort_DevInf0112:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>113</v>
       </c>
@@ -5385,7 +5415,7 @@
         <v>pPort_DevInf0113:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>114</v>
       </c>
@@ -5417,7 +5447,7 @@
         <v>pPort_DevInf0114:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>115</v>
       </c>
@@ -5449,7 +5479,7 @@
         <v>pPort_DevInf0115:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
         <v>116</v>
       </c>
@@ -5481,7 +5511,7 @@
         <v>pPort_DevInf0116:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>117</v>
       </c>
@@ -5513,7 +5543,7 @@
         <v>pPort_DevInf0117:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>118</v>
       </c>
@@ -5545,7 +5575,7 @@
         <v>pPort_DevInf0118:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -5577,7 +5607,7 @@
         <v>pPort_DevInf0119:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>120</v>
       </c>
@@ -5609,7 +5639,7 @@
         <v>pPort_DevInf0120:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>121</v>
       </c>
@@ -5641,7 +5671,7 @@
         <v>pPort_DevInf0121:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>122</v>
       </c>
@@ -5673,7 +5703,7 @@
         <v>pPort_DevInf0122:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>123</v>
       </c>
@@ -5705,7 +5735,7 @@
         <v>pPort_DevInf0123:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>124</v>
       </c>
@@ -5737,7 +5767,7 @@
         <v>pPort_DevInf0124:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
         <v>125</v>
       </c>
@@ -5769,7 +5799,7 @@
         <v>pPort_DevInf0125:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>126</v>
       </c>
@@ -5801,7 +5831,7 @@
         <v>pPort_DevInf0126:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
         <v>127</v>
       </c>
@@ -5833,7 +5863,7 @@
         <v>pPort_DevInf0127:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>128</v>
       </c>
@@ -5865,7 +5895,7 @@
         <v>pPort_DevInf0128:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
         <v>129</v>
       </c>
@@ -5897,7 +5927,7 @@
         <v>pPort_DevInf0129:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
         <v>130</v>
       </c>
@@ -5929,7 +5959,7 @@
         <v>pPort_DevInf0130:'pPort is NOT connected'</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -5938,7 +5968,7 @@
       <c r="F132"/>
       <c r="G132"/>
     </row>
-    <row r="133" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -5947,7 +5977,7 @@
       <c r="F133"/>
       <c r="G133"/>
     </row>
-    <row r="134" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -5956,7 +5986,7 @@
       <c r="F134"/>
       <c r="G134"/>
     </row>
-    <row r="135" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -5965,7 +5995,7 @@
       <c r="F135"/>
       <c r="G135"/>
     </row>
-    <row r="136" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -5974,7 +6004,7 @@
       <c r="F136"/>
       <c r="G136"/>
     </row>
-    <row r="137" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -5983,7 +6013,7 @@
       <c r="F137"/>
       <c r="G137"/>
     </row>
-    <row r="138" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -5993,7 +6023,7 @@
       <c r="G138"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J131"/>
+  <autoFilter ref="A1:J131" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -6003,861 +6033,861 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A149"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection activeCell="A145" sqref="A145:A148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.7421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
     </row>
-    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>CodeTable_Single_data!L2</f>
         <v>pPort_Err0001:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>CodeTable_Single_data!L3</f>
         <v>pPort_Err0002:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="13" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>CodeTable_Single_data!L4</f>
         <v>pPort_Err0003:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>CodeTable_Single_data!L5</f>
         <v>pPort_Err0004:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="15" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>CodeTable_Single_data!L6</f>
         <v>pPort_Err0005:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="16" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>CodeTable_Single_data!L7</f>
         <v>pPort_Err0006:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>CodeTable_Single_data!L8</f>
         <v>pPort_Err0007:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="18" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>CodeTable_Single_data!L9</f>
         <v>pPort_Err0008:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>CodeTable_Single_data!L10</f>
         <v>pPort_Err0009:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>CodeTable_Single_data!L11</f>
         <v>pPort_Err0010:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>CodeTable_Single_data!L12</f>
         <v>pPort_Err0011:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="22" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>CodeTable_Single_data!L13</f>
         <v>pPort_Err0012:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="23" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>CodeTable_Single_data!L14</f>
         <v>pPort_Err0013:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="24" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>CodeTable_Single_data!L15</f>
         <v>pPort_Err0014:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="25" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>CodeTable_Single_data!L16</f>
         <v>pPort_Err0015:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="26" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>CodeTable_Single_data!L17</f>
         <v>pPort_Err0016:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>CodeTable_Single_data!L18</f>
         <v>pPort_Err0017:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>CodeTable_Single_data!L19</f>
         <v>pPort_Err0018:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="29" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>CodeTable_Single_data!L20</f>
         <v>pPort_Err0019:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="30" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>CodeTable_Single_data!L21</f>
         <v>pPort_Err0020:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="31" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>CodeTable_Single_data!L22</f>
         <v>pPort_Warn0021:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="32" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>CodeTable_Single_data!L23</f>
         <v>pPort_Warn0022:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>CodeTable_Single_data!L24</f>
         <v>pPort_Warn0023:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>CodeTable_Single_data!L25</f>
         <v>pPort_Warn0024:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>CodeTable_Single_data!L26</f>
         <v>pPort_Warn0025:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>CodeTable_Single_data!L27</f>
         <v>pPort_Warn0026:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>CodeTable_Single_data!L28</f>
         <v>pPort_Warn0027:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>CodeTable_Single_data!L29</f>
         <v>pPort_Warn0028:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>CodeTable_Single_data!L30</f>
         <v>pPort_Warn0029:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>CodeTable_Single_data!L31</f>
         <v>pPort_Warn0030:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>CodeTable_Single_data!L32</f>
         <v>pPort_Warn0031:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>CodeTable_Single_data!L33</f>
         <v>pPort_Warn0032:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f>CodeTable_Single_data!L34</f>
         <v>pPort_Warn0033:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f>CodeTable_Single_data!L35</f>
         <v>pPort_Warn0034:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>CodeTable_Single_data!L36</f>
         <v>pPort_Warn0035:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f>CodeTable_Single_data!L37</f>
         <v>pPort_Warn0036:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>CodeTable_Single_data!L38</f>
         <v>pPort_Warn0037:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>CodeTable_Single_data!L39</f>
         <v>pPort_Warn0038:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>CodeTable_Single_data!L40</f>
         <v>pPort_Warn0039:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>CodeTable_Single_data!L41</f>
         <v>pPort_Warn0040:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>CodeTable_Single_data!L42</f>
         <v>pPort_Warn0041:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f>CodeTable_Single_data!L43</f>
         <v>pPort_Warn0042:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f>CodeTable_Single_data!L44</f>
         <v>pPort_Warn0043:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f>CodeTable_Single_data!L45</f>
         <v>pPort_Warn0044:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f>CodeTable_Single_data!L46</f>
         <v>pPort_Warn0045:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f>CodeTable_Single_data!L47</f>
         <v>pPort_Warn0046:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>CodeTable_Single_data!L48</f>
         <v>pPort_Warn0047:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f>CodeTable_Single_data!L49</f>
         <v>pPort_Warn0048:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f>CodeTable_Single_data!L50</f>
         <v>pPort_Warn0049:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f>CodeTable_Single_data!L51</f>
         <v>pPort_Warn0050:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f>CodeTable_Single_data!L52</f>
         <v>pPort_UsInf0051:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
         <f>CodeTable_Single_data!L53</f>
         <v>pPort_UsInf0052:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>CodeTable_Single_data!L54</f>
         <v>pPort_UsInf0053:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f>CodeTable_Single_data!L55</f>
         <v>pPort_UsInf0054:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f>CodeTable_Single_data!L56</f>
         <v>pPort_UsInf0055:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f>CodeTable_Single_data!L57</f>
         <v>pPort_UsInf0056:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f>CodeTable_Single_data!L58</f>
         <v>pPort_UsInf0057:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f>CodeTable_Single_data!L59</f>
         <v>pPort_UsInf0058:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>CodeTable_Single_data!L60</f>
         <v>pPort_UsInf0059:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f>CodeTable_Single_data!L61</f>
         <v>pPort_UsInf0060:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f>CodeTable_Single_data!L62</f>
         <v>pPort_UsInf0061:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f>CodeTable_Single_data!L63</f>
         <v>pPort_UsInf0062:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
         <f>CodeTable_Single_data!L64</f>
         <v>pPort_UsInf0063:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f>CodeTable_Single_data!L65</f>
         <v>pPort_UsInf0064:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f>CodeTable_Single_data!L66</f>
         <v>pPort_UsInf0065:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
         <f>CodeTable_Single_data!L67</f>
         <v>pPort_UsInf0066:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>CodeTable_Single_data!L68</f>
         <v>pPort_UsInf0067:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
         <f>CodeTable_Single_data!L69</f>
         <v>pPort_UsInf0068:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
         <f>CodeTable_Single_data!L70</f>
         <v>pPort_UsInf0069:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
         <f>CodeTable_Single_data!L71</f>
         <v>pPort_UsInf0070:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f>CodeTable_Single_data!L72</f>
         <v>pPort_UsInf0071:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
         <f>CodeTable_Single_data!L73</f>
         <v>pPort_UsInf0072:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f>CodeTable_Single_data!L74</f>
         <v>pPort_UsInf0073:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
         <f>CodeTable_Single_data!L75</f>
         <v>pPort_UsInf0074:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
         <f>CodeTable_Single_data!L76</f>
         <v>pPort_UsInf0075:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
         <f>CodeTable_Single_data!L77</f>
         <v>pPort_UsInf0076:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>CodeTable_Single_data!L78</f>
         <v>pPort_UsInf0077:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>CodeTable_Single_data!L79</f>
         <v>pPort_UsInf0078:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
         <f>CodeTable_Single_data!L80</f>
         <v>pPort_UsInf0079:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
         <f>CodeTable_Single_data!L81</f>
         <v>pPort_UsInf0080:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
         <f>CodeTable_Single_data!L82</f>
         <v>pPort_UsInf0081:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
         <f>CodeTable_Single_data!L83</f>
         <v>pPort_UsInf0082:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
         <f>CodeTable_Single_data!L84</f>
         <v>pPort_UsInf0083:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
         <f>CodeTable_Single_data!L85</f>
         <v>pPort_UsInf0084:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
         <f>CodeTable_Single_data!L86</f>
         <v>pPort_UsInf0085:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
         <f>CodeTable_Single_data!L87</f>
         <v>pPort_UsInf0086:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
         <f>CodeTable_Single_data!L88</f>
         <v>pPort_UsInf0087:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
         <f>CodeTable_Single_data!L89</f>
         <v>pPort_UsInf0088:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>CodeTable_Single_data!L90</f>
         <v>pPort_UsInf0089:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
         <f>CodeTable_Single_data!L91</f>
         <v>pPort_UsInf0090:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
         <f>CodeTable_Single_data!L92</f>
         <v>pPort_UsInf0091:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
         <f>CodeTable_Single_data!L93</f>
         <v>pPort_UsInf0092:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
         <f>CodeTable_Single_data!L94</f>
         <v>pPort_UsInf0093:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
         <f>CodeTable_Single_data!L95</f>
         <v>pPort_UsInf0094:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>CodeTable_Single_data!L96</f>
         <v>pPort_UsInf0095:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
         <f>CodeTable_Single_data!L97</f>
         <v>pPort_UsInf0096:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
         <f>CodeTable_Single_data!L98</f>
         <v>pPort_UsInf0097:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
         <f>CodeTable_Single_data!L99</f>
         <v>pPort_UsInf0098:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
         <f>CodeTable_Single_data!L100</f>
         <v>pPort_UsInf0099:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
         <f>CodeTable_Single_data!L101</f>
         <v>pPort_UsInf0100:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
         <f>CodeTable_Single_data!L102</f>
         <v>pPort_UsInf0101:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
         <f>CodeTable_Single_data!L103</f>
         <v>pPort_UsInf0102:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
         <f>CodeTable_Single_data!L104</f>
         <v>pPort_UsInf0103:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
         <f>CodeTable_Single_data!L105</f>
         <v>pPort_UsInf0104:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
         <f>CodeTable_Single_data!L106</f>
         <v>pPort_UsInf0105:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
         <f>CodeTable_Single_data!L107</f>
         <v>pPort_UsInf0106:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
         <f>CodeTable_Single_data!L108</f>
         <v>pPort_UsInf0107:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
         <f>CodeTable_Single_data!L109</f>
         <v>pPort_UsInf0108:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
         <f>CodeTable_Single_data!L110</f>
         <v>pPort_UsInf0109:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
         <f>CodeTable_Single_data!L111</f>
         <v>pPort_UsInf0110:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="str">
         <f>CodeTable_Single_data!L112</f>
         <v>pPort_DevInf0111:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="str">
         <f>CodeTable_Single_data!L113</f>
         <v>pPort_DevInf0112:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="str">
         <f>CodeTable_Single_data!L114</f>
         <v>pPort_DevInf0113:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="str">
         <f>CodeTable_Single_data!L115</f>
         <v>pPort_DevInf0114:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="str">
         <f>CodeTable_Single_data!L116</f>
         <v>pPort_DevInf0115:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="str">
         <f>CodeTable_Single_data!L117</f>
         <v>pPort_DevInf0116:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="str">
         <f>CodeTable_Single_data!L118</f>
         <v>pPort_DevInf0117:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="str">
         <f>CodeTable_Single_data!L119</f>
         <v>pPort_DevInf0118:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="str">
         <f>CodeTable_Single_data!L120</f>
         <v>pPort_DevInf0119:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="str">
         <f>CodeTable_Single_data!L121</f>
         <v>pPort_DevInf0120:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="str">
         <f>CodeTable_Single_data!L122</f>
         <v>pPort_DevInf0121:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="str">
         <f>CodeTable_Single_data!L123</f>
         <v>pPort_DevInf0122:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="str">
         <f>CodeTable_Single_data!L124</f>
         <v>pPort_DevInf0123:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="str">
         <f>CodeTable_Single_data!L125</f>
         <v>pPort_DevInf0124:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="str">
         <f>CodeTable_Single_data!L126</f>
         <v>pPort_DevInf0125:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="str">
         <f>CodeTable_Single_data!L127</f>
         <v>pPort_DevInf0126:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="str">
         <f>CodeTable_Single_data!L128</f>
         <v>pPort_DevInf0127:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="str">
         <f>CodeTable_Single_data!L129</f>
         <v>pPort_DevInf0128:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
         <f>CodeTable_Single_data!L130</f>
         <v>pPort_DevInf0129:'pPort is NOT connected',</v>
       </c>
     </row>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
         <f>CodeTable_Single_data!L131</f>
         <v>pPort_DevInf0130:'pPort is NOT connected'</v>
       </c>
     </row>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="24"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
         <f>CodeTable_Single_data!K2</f>
         <v>ERROR:{Err0001:{str:'Cannot connect to Operator. No Active Operator', data: tablePorts.pPort_Err0001},Err0002:{str:'Ip/Port is busy', data: tablePorts.pPort_Err0002},Err0003:{str:'Cannot process command', data: tablePorts.pPort_Err0003},Err0004:{str:'Error in configuration file', data: tablePorts.pPort_Err0004},Err0005:{str:'Invalid Count of Arguments', data: tablePorts.pPort_Err0005},Err0006:{str:'Invalid data from server (cannot be decrypted)', data: tablePorts.pPort_Err0006},Err0007:{str:'Invalid certificate excahange', data: tablePorts.pPort_Err0007},Err0008:{str:'Invalid digital address of operator', data: tablePorts.pPort_Err0008},Err0009:{str:'There is no active MySQL server on %s', data: tablePorts.pPort_Err0009},Err0010:{str:'', data: tablePorts.pPort_Err0010},Err0011:{str:'', data: tablePorts.pPort_Err0011},Err0012:{str:'', data: tablePorts.pPort_Err0012},Err0013:{str:'', data: tablePorts.pPort_Err0013},Err0014:{str:'', data: tablePorts.pPort_Err0014},Err0015:{str:'', data: tablePorts.pPort_Err0015},Err0016:{str:'', data: tablePorts.pPort_Err0016},Err0017:{str:'', data: tablePorts.pPort_Err0017},Err0018:{str:'', data: tablePorts.pPort_Err0018},Err0019:{str:'', data: tablePorts.pPort_Err0019},Err0020:{str:'', data: tablePorts.pPort_Err0020}},</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
         <f>CodeTable_Single_data!K22</f>
-        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'', data: tablePorts.pPort_Warn0031},Warn0032:{str:'', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+        <v>WARNING:{Warn0021:{str:'TCP Connection Closed', data: tablePorts.pPort_Warn0021},Warn0022:{str:'Client spontaneous disconnected.', data: tablePorts.pPort_Warn0022},Warn0023:{str:'Error DICE Unit has Invalid Value', data: tablePorts.pPort_Warn0023},Warn0024:{str:'Error Mismatch with Current Owner', data: tablePorts.pPort_Warn0024},Warn0025:{str:'Error New owner was already set', data: tablePorts.pPort_Warn0025},Warn0026:{str:'Error Mismatch New Owner field and requested address', data: tablePorts.pPort_Warn0026},Warn0027:{str:'Error Mismatch New Owner field and claimed owner', data: tablePorts.pPort_Warn0027},Warn0028:{str:'Error DICE Unit Exist in DB', data: tablePorts.pPort_Warn0028},Warn0029:{str:'Error Operator Address does not match with Operator Address in Prototype', data: tablePorts.pPort_Warn0029},Warn0030:{str:'Updating from cloud FAILED', data: tablePorts.pPort_Warn0030},Warn0031:{str:'Available units are insufficient for the amount', data: tablePorts.pPort_Warn0031},Warn0032:{str:'Unable to assemble the exact amount. Possible amount %s mDICE', data: tablePorts.pPort_Warn0032},Warn0033:{str:'', data: tablePorts.pPort_Warn0033},Warn0034:{str:'', data: tablePorts.pPort_Warn0034},Warn0035:{str:'', data: tablePorts.pPort_Warn0035},Warn0036:{str:'', data: tablePorts.pPort_Warn0036},Warn0037:{str:'', data: tablePorts.pPort_Warn0037},Warn0038:{str:'', data: tablePorts.pPort_Warn0038},Warn0039:{str:'', data: tablePorts.pPort_Warn0039},Warn0040:{str:'', data: tablePorts.pPort_Warn0040},Warn0041:{str:'', data: tablePorts.pPort_Warn0041},Warn0042:{str:'', data: tablePorts.pPort_Warn0042},Warn0043:{str:'', data: tablePorts.pPort_Warn0043},Warn0044:{str:'', data: tablePorts.pPort_Warn0044},Warn0045:{str:'', data: tablePorts.pPort_Warn0045},Warn0046:{str:'', data: tablePorts.pPort_Warn0046},Warn0047:{str:'', data: tablePorts.pPort_Warn0047},Warn0048:{str:'', data: tablePorts.pPort_Warn0048},Warn0049:{str:'', data: tablePorts.pPort_Warn0049},Warn0050:{str:'', data: tablePorts.pPort_Warn0050}},</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
         <f>CodeTable_Single_data!K52</f>
-        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+        <v>USER_INFO:{UsInf0051:{str:'User settings for value of new DICE Unit: %s', data: tablePorts.pPort_UsInf0051},UsInf0052:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0052},UsInf0053:{str:'Generating new Digital Address and Key Pair', data: tablePorts.pPort_UsInf0053},UsInf0054:{str:'Exit from Program', data: tablePorts.pPort_UsInf0054},UsInf0055:{str:'SHA3 Speed [hash/s]: %s ', data: tablePorts.pPort_UsInf0055},UsInf0056:{str:'Calculate new DICE Unit with Level - %s Operator Threshold', data: tablePorts.pPort_UsInf0056},UsInf0057:{str:'Saving generated Unit to %s', data: tablePorts.pPort_UsInf0057},UsInf0058:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0058},UsInf0059:{str:'Base 58 Key:  %s', data: tablePorts.pPort_UsInf0059},UsInf0060:{str:'Base 58 Addr: %s', data: tablePorts.pPort_UsInf0060},UsInf0061:{str:'Unit Content in HEX', data: tablePorts.pPort_UsInf0061},UsInf0062:{str:'Operator Address: %s', data: tablePorts.pPort_UsInf0062},UsInf0063:{str:'Miner Address: %s', data: tablePorts.pPort_UsInf0063},UsInf0064:{str:'Traling Zeroes:  %s', data: tablePorts.pPort_UsInf0064},UsInf0065:{str:'Time: %s', data: tablePorts.pPort_UsInf0065},UsInf0066:{str:'Payload: %s', data: tablePorts.pPort_UsInf0066},UsInf0067:{str:'Operator Response Message', data: tablePorts.pPort_UsInf0067},UsInf0068:{str:'Response Status: %s', data: tablePorts.pPort_UsInf0068},UsInf0069:{str:'Current Owner: %s', data: tablePorts.pPort_UsInf0069},UsInf0070:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0070},UsInf0071:{str:'Hash value of Prototype: %s', data: tablePorts.pPort_UsInf0071},UsInf0072:{str:'End of Operator Response Message', data: tablePorts.pPort_UsInf0072},UsInf0073:{str:'DICE Unit successfully registered in Data Base', data: tablePorts.pPort_UsInf0073},UsInf0074:{str:'DICE Value: %s', data: tablePorts.pPort_UsInf0074},UsInf0075:{str:'Claim accepted!', data: tablePorts.pPort_UsInf0075},UsInf0076:{str:'New owner accepted!', data: tablePorts.pPort_UsInf0076},UsInf0077:{str:'New configuration applied at: %s', data: tablePorts.pPort_UsInf0077},UsInf0078:{str:'Operator Threshold: %s ', data: tablePorts.pPort_UsInf0078},UsInf0079:{str:'Global Threshold: %s', data: tablePorts.pPort_UsInf0079},UsInf0080:{str:'Digital Address: %s', data: tablePorts.pPort_UsInf0080},UsInf0081:{str:'IP: %s', data: tablePorts.pPort_UsInf0081},UsInf0082:{str:'Port: %s', data: tablePorts.pPort_UsInf0082},UsInf0083:{str:'Operator Running', data: tablePorts.pPort_UsInf0083},UsInf0084:{str:'New added Unit %s', data: tablePorts.pPort_UsInf0084},UsInf0085:{str:'Imported configration', data: tablePorts.pPort_UsInf0085},UsInf0086:{str:'New Contact Added', data: tablePorts.pPort_UsInf0086},UsInf0087:{str:'New Operator Added', data: tablePorts.pPort_UsInf0087},UsInf0088:{str:'Created New configration file', data: tablePorts.pPort_UsInf0088},UsInf0089:{str:'DNS Updated', data: tablePorts.pPort_UsInf0089},UsInf0090:{str:'Balance %s', data: tablePorts.pPort_UsInf0090},UsInf0091:{str:'DICE Scrapped unit successfully registered ', data: tablePorts.pPort_UsInf0091},UsInf0092:{str:'You want to trade %s mDICE', data: tablePorts.pPort_UsInf0092},UsInf0093:{str:'All units are packed', data: tablePorts.pPort_UsInf0093},UsInf0094:{str:'', data: tablePorts.pPort_UsInf0094},UsInf0095:{str:'', data: tablePorts.pPort_UsInf0095},UsInf0096:{str:'', data: tablePorts.pPort_UsInf0096},UsInf0097:{str:'', data: tablePorts.pPort_UsInf0097},UsInf0098:{str:'', data: tablePorts.pPort_UsInf0098},UsInf0099:{str:'', data: tablePorts.pPort_UsInf0099},UsInf0100:{str:'', data: tablePorts.pPort_UsInf0100},UsInf0101:{str:'', data: tablePorts.pPort_UsInf0101},UsInf0102:{str:'', data: tablePorts.pPort_UsInf0102},UsInf0103:{str:'', data: tablePorts.pPort_UsInf0103},UsInf0104:{str:'', data: tablePorts.pPort_UsInf0104},UsInf0105:{str:'', data: tablePorts.pPort_UsInf0105},UsInf0106:{str:'', data: tablePorts.pPort_UsInf0106},UsInf0107:{str:'', data: tablePorts.pPort_UsInf0107},UsInf0108:{str:'', data: tablePorts.pPort_UsInf0108},UsInf0109:{str:'', data: tablePorts.pPort_UsInf0109},UsInf0110:{str:'', data: tablePorts.pPort_UsInf0110}},</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>CodeTable_Single_data!K112</f>
         <v>DEV_INFO:{DevInf0111:{str:'Base Hex Key:  %s', data: tablePorts.pPort_DevInf0111},DevInf0112:{str:'Base Hex Addr: %s', data: tablePorts.pPort_DevInf0112},DevInf0113:{str:'Data received: %s', data: tablePorts.pPort_DevInf0113},DevInf0114:{str:'', data: tablePorts.pPort_DevInf0114},DevInf0115:{str:'', data: tablePorts.pPort_DevInf0115},DevInf0116:{str:'', data: tablePorts.pPort_DevInf0116},DevInf0117:{str:'', data: tablePorts.pPort_DevInf0117},DevInf0118:{str:'', data: tablePorts.pPort_DevInf0118},DevInf0119:{str:'', data: tablePorts.pPort_DevInf0119},DevInf0120:{str:'', data: tablePorts.pPort_DevInf0120},DevInf0121:{str:'', data: tablePorts.pPort_DevInf0121},DevInf0122:{str:'', data: tablePorts.pPort_DevInf0122},DevInf0123:{str:'', data: tablePorts.pPort_DevInf0123},DevInf0124:{str:'', data: tablePorts.pPort_DevInf0124},DevInf0125:{str:'', data: tablePorts.pPort_DevInf0125},DevInf0126:{str:'', data: tablePorts.pPort_DevInf0126},DevInf0127:{str:'', data: tablePorts.pPort_DevInf0127},DevInf0128:{str:'', data: tablePorts.pPort_DevInf0128},DevInf0129:{str:'', data: tablePorts.pPort_DevInf0129},DevInf0130:{str:'', data: tablePorts.pPort_DevInf0130}}</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>290</v>
       </c>
@@ -6869,31 +6899,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="12.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.2265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="2"/>
+    <col min="3" max="3" width="12.10546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.76171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.5078125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48" customWidth="1"/>
-    <col min="9" max="9" width="38.44140625" customWidth="1"/>
-    <col min="10" max="10" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="125.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.0234375" customWidth="1"/>
+    <col min="9" max="9" width="38.47265625" customWidth="1"/>
+    <col min="10" max="10" width="43.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="35.37890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="125.2421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6934,7 +6964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -6966,7 +6996,7 @@
         <v>Err0001: { str:'Cannot connect to Operator. No Active Operator',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -6998,7 +7028,7 @@
         <v>Err0002: { str:'Ip/Port is busy',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -7030,7 +7060,7 @@
         <v>Err0003: { str:'Cannot process command',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -7062,7 +7092,7 @@
         <v>Err0004: { str:'Error in configuration file',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -7088,7 +7118,7 @@
         <v>Err0005: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -7114,7 +7144,7 @@
         <v>Err0006: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -7140,7 +7170,7 @@
         <v>Err0007: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -7166,7 +7196,7 @@
         <v>Err0008: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -7192,7 +7222,7 @@
         <v>Err0009: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -7218,7 +7248,7 @@
         <v>Err0010: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -7250,7 +7280,7 @@
         <v>Warn0011: { str:'TCP Connection Closed',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -7282,7 +7312,7 @@
         <v>Warn0012: { str:'Client spontaneous disconnected.',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -7314,7 +7344,7 @@
         <v>Warn0013: { str:'Error DICE Unit has Invalid Value',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -7346,7 +7376,7 @@
         <v>Warn0014: { str:'Error Mismatch with Current Owner',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -7378,7 +7408,7 @@
         <v>Warn0015: { str:'Error New owner was already set',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -7410,7 +7440,7 @@
         <v>Warn0016: { str:'Error Mismatch New Owner field and requested address',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -7442,7 +7472,7 @@
         <v>Warn0017: { str:'Error Mismatch New Owner field and claimed owner',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -7467,7 +7497,7 @@
         <v>Warn0018: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -7493,7 +7523,7 @@
         <v>Warn0019: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -7519,7 +7549,7 @@
         <v>Warn0020: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -7551,7 +7581,7 @@
         <v>UsInf0021: { str:'User settings for value of new DICE Unit: %s',plch:[()=&gt;{return Args.spareCommand;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -7583,7 +7613,7 @@
         <v>UsInf0022: { str:'DICE Value: %s',plch:[()=&gt;{return DICEValue.unitValue;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -7615,7 +7645,7 @@
         <v>UsInf0023: { str:'Generating new Digital Address and Key Pair',plch:[()=&gt;{return undefined;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -7647,7 +7677,7 @@
         <v>UsInf0024: { str:'Exit from Program',plch:[()=&gt;{return undefined;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -7679,7 +7709,7 @@
         <v>UsInf0025: { str:'SHA3 Speed: %s hash/s',plch:[()=&gt;{return DiceCalculatorL.getSHA3Count() ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -7711,7 +7741,7 @@
         <v>UsInf0026: { str:'Calculate new DICE Unit with Level - %s Operator Threshold',plch:[()=&gt;{return zeroes;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -7743,7 +7773,7 @@
         <v>UsInf0027: { str:'Saving generated Unit to %s',plch:[()=&gt;{return fileOutput;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -7775,7 +7805,7 @@
         <v>UsInf0028: { str:'Hash value of Prototype: %s',plch:[()=&gt;{return DiceCalculatorL.getSHA3OfUnit(DICE);},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -7805,7 +7835,7 @@
         <v>UsInf0029: { str:'Operator Running',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -7837,7 +7867,7 @@
         <v>UsInf0030: { str:'Base 58 Key:  %s',plch:[()=&gt;{return keyPair.privateKey;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -7869,7 +7899,7 @@
         <v>UsInf0031: { str:'Base 58 Addr: %s',plch:[()=&gt;{return keyPair.digitalAddress;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -7903,7 +7933,7 @@
         <v>UsInf0032: { str:'Operator Params: Operator Threshold: %s  Global Threshold: %s',plch:[()=&gt;{return zeroes;},()=&gt;{return valData.N;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -7939,7 +7969,7 @@
         <v>UsInf0033: { str:'%s %s %s',plch:[()=&gt;{return keyPair.digitalAddress;},()=&gt;{return OperatorData.ip;},()=&gt;{return OperatorData.port;}]},</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -7971,7 +8001,7 @@
         <v>UsInf0034: { str:'Unit Content in HEX',plch:[()=&gt;{return undefined;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -8003,7 +8033,7 @@
         <v>UsInf0035: { str:'Operator Address: %s',plch:[()=&gt;{return Buffer.from(DICE.addrOperator.buffer).toString('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -8035,7 +8065,7 @@
         <v>UsInf0036: { str:'Miner Address: %s',plch:[()=&gt;{return Buffer.from(DICE.addrMiner.buffer).toString('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -8067,7 +8097,7 @@
         <v>UsInf0037: { str:'Traling Zeroes:  %s',plch:[()=&gt;{return Buffer.from(DICE.validZeros.buffer).toString('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -8099,7 +8129,7 @@
         <v>UsInf0038: { str:'Time: %s',plch:[()=&gt;{return Buffer.from(DICE.swatchTime.buffer).toString('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -8131,7 +8161,7 @@
         <v>UsInf0039: { str:'Payload: %s',plch:[()=&gt;{return Buffer.from(DICE.payLoad.buffer).toString('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -8161,7 +8191,7 @@
         <v>UsInf0040: { str:'\nOperator Response Message',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -8193,7 +8223,7 @@
         <v>UsInf0041: { str:'Response Status: %s',plch:[()=&gt;{return response.status.toString();},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -8225,7 +8255,7 @@
         <v>UsInf0042: { str:'Current Owner: %s',plch:[()=&gt;{return response.data.curOwner;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -8257,7 +8287,7 @@
         <v>UsInf0043: { str:'DICE Value: %s',plch:[()=&gt;{return response.data.diceValue;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -8289,7 +8319,7 @@
         <v>UsInf0044: { str:'Hash value of Prototype: %s',plch:[()=&gt;{return response.data.hash;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -8321,7 +8351,7 @@
         <v>UsInf0045: { str:'End of Operator Response Message \n',plch:[()=&gt;{return undefined;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -8351,7 +8381,7 @@
         <v>UsInf0046: { str:'DICE Unit successfully registered in Data Base',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -8383,7 +8413,7 @@
         <v>UsInf0047: { str:'DICE Value: %s',plch:[()=&gt;{return DICEValue.unitValue;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -8413,7 +8443,7 @@
         <v>UsInf0048: { str:'Claim accepted!',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -8443,7 +8473,7 @@
         <v>UsInf0049: { str:'New owner accepted!',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -8475,7 +8505,7 @@
         <v>UsInf0050: { str:'New configuration applied at: %s',plch:[()=&gt;{return curr.mtime;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -8501,7 +8531,7 @@
         <v>UsInf0051: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -8527,7 +8557,7 @@
         <v>UsInf0052: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -8561,7 +8591,7 @@
         <v>DevInf0053: { str:'Base Hex Key:  %s',plch:[()=&gt;{return AddressGen.getPrivateKey('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -8595,7 +8625,7 @@
         <v>DevInf0054: { str:'Base Hex Addr: %s',plch:[()=&gt;{return AddressGen.getDigitalAdress('hex');},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -8629,7 +8659,7 @@
         <v>DevInf0055: { str:'Data received: %s',plch:[()=&gt;{return data.toString();},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -8655,7 +8685,7 @@
         <v>DevInf0056: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -8681,7 +8711,7 @@
         <v>DevInf0057: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -8707,7 +8737,7 @@
         <v>DevInf0058: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -8733,7 +8763,7 @@
         <v>DevInf0059: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -8759,7 +8789,7 @@
         <v>DevInf0060: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -8785,7 +8815,7 @@
         <v>DevInf0061: { str:'',plch:[()=&gt;{return ;},()=&gt;{return ;},()=&gt;{return ;}]},</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -8812,7 +8842,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I63"/>
+  <autoFilter ref="A1:I63" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -8822,20 +8852,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="63" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.0625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="62.95703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -8847,7 +8877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -8859,7 +8889,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -8871,7 +8901,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -8883,7 +8913,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -8895,7 +8925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -8907,7 +8937,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -8919,7 +8949,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -8931,7 +8961,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -8943,7 +8973,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -8955,7 +8985,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -8967,7 +8997,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -8979,7 +9009,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -8991,7 +9021,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -9003,7 +9033,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -9015,7 +9045,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -9027,7 +9057,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -9039,7 +9069,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -9051,7 +9081,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -9063,7 +9093,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -9075,7 +9105,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -9087,7 +9117,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -9099,7 +9129,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -9111,7 +9141,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -9123,7 +9153,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>

</xml_diff>